<commit_message>
fixing some issues in part 1b
</commit_message>
<xml_diff>
--- a/data/data_digitization/occurrence_data/1_raw_data/HJ-27-occ-entry.xlsx
+++ b/data/data_digitization/occurrence_data/1_raw_data/HJ-27-occ-entry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/occurrence_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13128257-1355-614F-8D78-CF25C2386D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1E15F3-2E60-664E-9CE8-1617DDEF260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15400" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3394,7 +3394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3682,7 +3682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3692,10 +3692,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="157" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="Q94" sqref="Q94"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8055,6 +8055,9 @@
       <c r="A87" s="4">
         <v>5</v>
       </c>
+      <c r="B87" s="4">
+        <v>5</v>
+      </c>
       <c r="C87" s="4" t="s">
         <v>217</v>
       </c>
@@ -8093,6 +8096,9 @@
       <c r="A88" s="4">
         <v>5</v>
       </c>
+      <c r="B88" s="4">
+        <v>6</v>
+      </c>
       <c r="C88" s="4" t="s">
         <v>220</v>
       </c>
@@ -8131,6 +8137,9 @@
       <c r="A89" s="4">
         <v>5</v>
       </c>
+      <c r="B89" s="4">
+        <v>7</v>
+      </c>
       <c r="C89" s="4" t="s">
         <v>223</v>
       </c>
@@ -8169,6 +8178,9 @@
       <c r="A90" s="4">
         <v>5</v>
       </c>
+      <c r="B90" s="4">
+        <v>8</v>
+      </c>
       <c r="C90" s="4" t="s">
         <v>226</v>
       </c>
@@ -8201,6 +8213,9 @@
       <c r="A91" s="4">
         <v>5</v>
       </c>
+      <c r="B91" s="4">
+        <v>9</v>
+      </c>
       <c r="C91" s="4" t="s">
         <v>230</v>
       </c>
@@ -8239,6 +8254,9 @@
       <c r="A92" s="4">
         <v>5</v>
       </c>
+      <c r="B92" s="4">
+        <v>10</v>
+      </c>
       <c r="C92" s="4" t="s">
         <v>188</v>
       </c>
@@ -8277,6 +8295,9 @@
       <c r="A93" s="4">
         <v>5</v>
       </c>
+      <c r="B93" s="4">
+        <v>11</v>
+      </c>
       <c r="C93" s="4" t="s">
         <v>38</v>
       </c>
@@ -8315,6 +8336,9 @@
       <c r="A94" s="4">
         <v>5</v>
       </c>
+      <c r="B94" s="4">
+        <v>12</v>
+      </c>
       <c r="C94" s="4" t="s">
         <v>232</v>
       </c>
@@ -8356,6 +8380,9 @@
       <c r="A95" s="4">
         <v>5</v>
       </c>
+      <c r="B95" s="4">
+        <v>13</v>
+      </c>
       <c r="C95" s="4" t="s">
         <v>56</v>
       </c>
@@ -8394,6 +8421,9 @@
       <c r="A96" s="4">
         <v>5</v>
       </c>
+      <c r="B96" s="4">
+        <v>14</v>
+      </c>
       <c r="C96" s="4" t="s">
         <v>235</v>
       </c>
@@ -8432,6 +8462,9 @@
       <c r="A97" s="4">
         <v>5</v>
       </c>
+      <c r="B97" s="4">
+        <v>15</v>
+      </c>
       <c r="C97" s="4" t="s">
         <v>237</v>
       </c>
@@ -8470,6 +8503,9 @@
       <c r="A98" s="4">
         <v>5</v>
       </c>
+      <c r="B98" s="4">
+        <v>16</v>
+      </c>
       <c r="C98" s="4" t="s">
         <v>238</v>
       </c>
@@ -8508,6 +8544,9 @@
       <c r="A99" s="4">
         <v>5</v>
       </c>
+      <c r="B99" s="4">
+        <v>17</v>
+      </c>
       <c r="C99" s="4" t="s">
         <v>194</v>
       </c>
@@ -8546,6 +8585,9 @@
       <c r="A100" s="4">
         <v>5</v>
       </c>
+      <c r="B100" s="4">
+        <v>18</v>
+      </c>
       <c r="C100" s="4" t="s">
         <v>239</v>
       </c>
@@ -8584,6 +8626,9 @@
       <c r="A101" s="4">
         <v>5</v>
       </c>
+      <c r="B101" s="4">
+        <v>19</v>
+      </c>
       <c r="C101" s="4" t="s">
         <v>25</v>
       </c>
@@ -8621,6 +8666,9 @@
     <row r="102" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>5</v>
+      </c>
+      <c r="B102" s="4">
+        <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>241</v>

</xml_diff>